<commit_message>
updated excel test data file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DsAlgo_ExcelData.xlsx
+++ b/src/test/resources/testdata/DsAlgo_ExcelData.xlsx
@@ -33,13 +33,13 @@
     <t>Message</t>
   </si>
   <si>
-    <t>newuser123</t>
+    <t>newuser456</t>
   </si>
   <si>
     <t>testpassword1</t>
   </si>
   <si>
-    <t>New Account Created. You are logged in as qazw</t>
+    <t>New Account Created. You are logged in as newuser456</t>
   </si>
   <si>
     <t>TT1234$#@!</t>
@@ -433,7 +433,7 @@
     <col customWidth="1" min="1" max="1" width="11.63"/>
     <col customWidth="1" min="2" max="2" width="12.88"/>
     <col customWidth="1" min="3" max="3" width="15.63"/>
-    <col customWidth="1" min="4" max="4" width="39.0"/>
+    <col customWidth="1" min="4" max="4" width="41.88"/>
     <col customWidth="1" min="5" max="6" width="10.88"/>
     <col customWidth="1" min="7" max="26" width="10.63"/>
   </cols>
@@ -484,7 +484,7 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1"/>

</xml_diff>